<commit_message>
Add Bernard lake station
</commit_message>
<xml_diff>
--- a/Resources/Metadata.xlsx
+++ b/Resources/Metadata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/anthi182_ulaval_ca/Documents/Documents/GitHub/Ro2_data_worflow/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="13_ncr:1_{DD6382FE-130C-4706-8590-2E836291513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10CA2BEC-F7CB-4DF4-B53D-DD6942BA1B11}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="13_ncr:1_{DD6382FE-130C-4706-8590-2E836291513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B01B1D07-6996-4435-8564-B0924EBCFFAD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
   </bookViews>
   <sheets>
     <sheet name="Berge" sheetId="3" r:id="rId1"/>
-    <sheet name="Bernard" sheetId="8" r:id="rId2"/>
+    <sheet name="Bernard_lake" sheetId="8" r:id="rId2"/>
     <sheet name="Foret" sheetId="5" r:id="rId3"/>
     <sheet name="Reservoir" sheetId="4" r:id="rId4"/>
     <sheet name="Thermistors" sheetId="6" r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
   <si>
     <t>Instrument</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Distance between instruments (sonic as reference) in cm</t>
+  </si>
+  <si>
+    <t>Thermistors chain 1</t>
   </si>
 </sst>
 </file>
@@ -1146,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE44D4E6-1DC8-5846-9613-DEB0E908B686}">
   <dimension ref="B1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1322,7 +1325,7 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1347,7 +1350,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="22">
-        <v>50.861590999999997</v>
+        <v>50.861454700000003</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -1364,7 +1367,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="2">
-        <v>-63.389947999999997</v>
+        <v>-63.389840900000003</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
@@ -1476,10 +1479,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="39">
-        <v>-35</v>
+        <v>-37.5</v>
       </c>
       <c r="D17" s="14">
-        <v>15</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -1496,7 +1499,7 @@
   <dimension ref="B1:G27"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1879,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53111C9A-58C1-40C7-9383-CFE5F1F570E0}">
   <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1894,7 +1897,7 @@
     <row r="1" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="63" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C2" s="64"/>
       <c r="E2" s="63" t="s">

</xml_diff>

<commit_message>
Add gap filling for Bernard Lake
</commit_message>
<xml_diff>
--- a/Resources/Metadata.xlsx
+++ b/Resources/Metadata.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/anthi182_ulaval_ca/Documents/Documents/GitHub/Ro2_data_worflow/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="13_ncr:1_{DD6382FE-130C-4706-8590-2E836291513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B01B1D07-6996-4435-8564-B0924EBCFFAD}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="13_ncr:1_{DD6382FE-130C-4706-8590-2E836291513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA390F7-3144-4AD5-96A6-B39F9EC0D2FA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
   </bookViews>
   <sheets>
     <sheet name="Berge" sheetId="3" r:id="rId1"/>
     <sheet name="Bernard_lake" sheetId="8" r:id="rId2"/>
     <sheet name="Foret" sheetId="5" r:id="rId3"/>
     <sheet name="Reservoir" sheetId="4" r:id="rId4"/>
-    <sheet name="Thermistors" sheetId="6" r:id="rId5"/>
-    <sheet name="Natashquan" sheetId="7" r:id="rId6"/>
+    <sheet name="Romaine-2 thermistors" sheetId="6" r:id="rId5"/>
+    <sheet name="Bernard lake thermistors" sheetId="9" r:id="rId6"/>
+    <sheet name="Natashquan" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="55">
   <si>
     <t>Instrument</t>
   </si>
@@ -200,6 +201,12 @@
   </si>
   <si>
     <t>Thermistors chain 1</t>
+  </si>
+  <si>
+    <t>Thermistors chain</t>
+  </si>
+  <si>
+    <t>HOBO MX2202</t>
   </si>
 </sst>
 </file>
@@ -743,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -760,28 +767,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
@@ -791,20 +793,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1164,15 +1166,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1181,13 +1183,13 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="30" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="15" t="s">
@@ -1198,19 +1200,19 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="27">
         <v>8</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="28">
         <v>7.25</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1218,92 +1220,92 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="27">
         <v>7.25</v>
       </c>
       <c r="D6" s="13"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <v>7.25</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="27">
         <v>6.3</v>
       </c>
       <c r="D8" s="13"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <v>5.2</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="35" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="27">
         <v>2.2999999999999998</v>
       </c>
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="28">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="34">
         <v>0.9</v>
       </c>
       <c r="D12" s="14"/>
     </row>
     <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-    </row>
-    <row r="16" spans="2:7" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="32"/>
-      <c r="C16" s="28" t="s">
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
+    </row>
+    <row r="16" spans="2:7" s="36" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="29"/>
+      <c r="C16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="34">
         <v>24</v>
       </c>
       <c r="D17" s="14">
@@ -1336,17 +1338,14 @@
     <col min="7" max="7" width="14.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-    </row>
+    <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="F2" s="37" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="22">
@@ -1354,16 +1353,16 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="38" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="2">
@@ -1371,19 +1370,19 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="27">
         <v>0.8</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="28">
         <v>4.3</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1391,28 +1390,28 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="27">
         <v>4.3</v>
       </c>
       <c r="D6" s="13"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="28">
         <v>4.3</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="27">
         <v>3.9</v>
       </c>
       <c r="D8" s="13" t="s">
@@ -1420,65 +1419,65 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="28">
         <v>0.8</v>
       </c>
-      <c r="D9" s="40"/>
+      <c r="D9" s="35"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="27">
         <v>2</v>
       </c>
       <c r="D10" s="13"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="28">
         <v>1.2</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="34">
         <v>1</v>
       </c>
       <c r="D12" s="14"/>
     </row>
     <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="32"/>
-      <c r="C16" s="28" t="s">
+      <c r="B16" s="29"/>
+      <c r="C16" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="34">
         <v>-37.5</v>
       </c>
       <c r="D17" s="14">
@@ -1511,26 +1510,26 @@
   <sheetData>
     <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="F2" s="55" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="F2" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="56">
+      <c r="G2" s="51">
         <v>50.9020996</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="30" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="15" t="s">
@@ -1541,182 +1540,182 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="27">
         <v>24</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:7" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="48">
         <v>24</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="49" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="44">
         <v>-0.03</v>
       </c>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="48">
+      <c r="C7" s="43">
         <v>24</v>
       </c>
       <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="44">
         <v>24</v>
       </c>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="43">
         <v>-0.1</v>
       </c>
       <c r="D9" s="16"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="44">
         <v>24</v>
       </c>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="48">
+      <c r="C11" s="43">
         <v>20</v>
       </c>
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="44">
         <v>15</v>
       </c>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="48">
+      <c r="C13" s="43">
         <v>10</v>
       </c>
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="44">
         <v>5</v>
       </c>
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="43">
         <v>26</v>
       </c>
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="44">
         <v>24</v>
       </c>
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="43">
         <v>25</v>
       </c>
       <c r="D17" s="16"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="44">
         <v>25</v>
       </c>
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="48">
+      <c r="C19" s="43">
         <v>-0.03</v>
       </c>
       <c r="D19" s="16"/>
     </row>
     <row r="20" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="50">
+      <c r="C20" s="45">
         <v>-0.09</v>
       </c>
-      <c r="D20" s="25"/>
+      <c r="D20" s="24"/>
     </row>
     <row r="22" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="59"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="32"/>
-      <c r="C24" s="28" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="27">
         <v>10</v>
       </c>
       <c r="D25" s="13">
@@ -1724,10 +1723,10 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="48">
+      <c r="C26" s="43">
         <v>6.5</v>
       </c>
       <c r="D26" s="16">
@@ -1735,10 +1734,10 @@
       </c>
     </row>
     <row r="27" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="51" t="s">
+      <c r="B27" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="39">
+      <c r="C27" s="34">
         <v>-10</v>
       </c>
       <c r="D27" s="12">
@@ -1771,15 +1770,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1788,13 +1787,13 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="30" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="15" t="s">
@@ -1805,10 +1804,10 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="27">
         <v>1.5</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -1816,52 +1815,52 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="28">
         <v>2</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="34">
         <v>2</v>
       </c>
       <c r="D6" s="14"/>
     </row>
     <row r="8" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="32"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="29"/>
+      <c r="C10" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="34">
         <v>85</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="34">
         <v>-10</v>
       </c>
       <c r="E11" s="14">
@@ -1882,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53111C9A-58C1-40C7-9383-CFE5F1F570E0}">
   <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1896,14 +1895,14 @@
   <sheetData>
     <row r="1" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="E2" s="63" t="s">
+      <c r="C2" s="59"/>
+      <c r="E2" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="64"/>
+      <c r="F2" s="59"/>
     </row>
     <row r="3" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="18" t="s">
@@ -2208,8 +2207,8 @@
       </c>
     </row>
     <row r="25" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
       <c r="E25" s="9" t="s">
         <v>19</v>
       </c>
@@ -2302,8 +2301,8 @@
       </c>
     </row>
     <row r="36" spans="5:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
     </row>
     <row r="37" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E37" s="7" t="s">
@@ -2331,6 +2330,227 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BF41A8-026E-451A-9D63-213454538E4C}">
+  <dimension ref="B1:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="59"/>
+    </row>
+    <row r="3" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="13">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="14">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="8">
+        <v>50.860754999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3">
+        <v>-63.389910999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EED9BCF-AC84-402D-B7FA-16D351A40D85}">
   <dimension ref="B1:C7"/>
   <sheetViews>
@@ -2345,10 +2565,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="64"/>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">
@@ -2367,10 +2587,10 @@
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Bernard spruce moss metadata
</commit_message>
<xml_diff>
--- a/Resources/Metadata.xlsx
+++ b/Resources/Metadata.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/anthi182_ulaval_ca/Documents/Documents/GitHub/Ro2_data_worflow/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="289" documentId="13_ncr:1_{DD6382FE-130C-4706-8590-2E836291513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DA390F7-3144-4AD5-96A6-B39F9EC0D2FA}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="13_ncr:1_{DD6382FE-130C-4706-8590-2E836291513C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC4DEE56-65E6-492E-A5E1-25375DE742FF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
+    <workbookView minimized="1" xWindow="29940" yWindow="1140" windowWidth="21600" windowHeight="11175" activeTab="3" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
   </bookViews>
   <sheets>
     <sheet name="Berge" sheetId="3" r:id="rId1"/>
     <sheet name="Bernard_lake" sheetId="8" r:id="rId2"/>
     <sheet name="Foret" sheetId="5" r:id="rId3"/>
-    <sheet name="Reservoir" sheetId="4" r:id="rId4"/>
-    <sheet name="Romaine-2 thermistors" sheetId="6" r:id="rId5"/>
-    <sheet name="Bernard lake thermistors" sheetId="9" r:id="rId6"/>
-    <sheet name="Natashquan" sheetId="7" r:id="rId7"/>
+    <sheet name="Foret_neige" sheetId="11" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="10" r:id="rId5"/>
+    <sheet name="Reservoir" sheetId="4" r:id="rId6"/>
+    <sheet name="Romaine-2 thermistors" sheetId="6" r:id="rId7"/>
+    <sheet name="Bernard lake thermistors" sheetId="9" r:id="rId8"/>
+    <sheet name="Natashquan" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="87">
   <si>
     <t>Instrument</t>
   </si>
@@ -207,13 +209,109 @@
   </si>
   <si>
     <t>HOBO MX2202</t>
+  </si>
+  <si>
+    <t>(-25, -15)</t>
+  </si>
+  <si>
+    <t>Vol. liquid water content (0 -1)</t>
+  </si>
+  <si>
+    <t>HMP60</t>
+  </si>
+  <si>
+    <t>Relative humidity (%)</t>
+  </si>
+  <si>
+    <t>Air temp. (°C)</t>
+  </si>
+  <si>
+    <t>Si-111</t>
+  </si>
+  <si>
+    <t>Snow surf. temp. (°C)</t>
+  </si>
+  <si>
+    <t>(0, 15, 30, 45, 60, 75, 90, 105, 120)</t>
+  </si>
+  <si>
+    <t>Pt-1000 thermistor</t>
+  </si>
+  <si>
+    <t>Snow temp. (°C)</t>
+  </si>
+  <si>
+    <t>(-0.2, -0.1, -0.05)</t>
+  </si>
+  <si>
+    <t>Soil temp. (°C)</t>
+  </si>
+  <si>
+    <t>SR50</t>
+  </si>
+  <si>
+    <t>snow height (m)</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>(0, 15, 30, 45, 60, 75, 90, 105, 120, 135, 150)</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>(0, 15, 30, 45, 60, 75, 90, 105, 120, 135)</t>
+  </si>
+  <si>
+    <t>2020-2021</t>
+  </si>
+  <si>
+    <t>Judd communication sensor</t>
+  </si>
+  <si>
+    <t>snow height (cm)</t>
+  </si>
+  <si>
+    <t>2019-2020</t>
+  </si>
+  <si>
+    <t>Gap</t>
+  </si>
+  <si>
+    <t>(0, 15, 30, 45, 60, 75)</t>
+  </si>
+  <si>
+    <t>(0, 15, 30, 45, 60, 75, 90, 105)</t>
+  </si>
+  <si>
+    <t>(0, 15, 30, 45, 60, 75, 90)</t>
+  </si>
+  <si>
+    <t>SR50A</t>
+  </si>
+  <si>
+    <t>Canopy</t>
+  </si>
+  <si>
+    <t>height (m)</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,6 +321,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -254,7 +367,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -746,11 +859,232 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -811,6 +1145,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -819,6 +1174,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -852,10 +1234,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -893,7 +1279,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -999,7 +1385,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1141,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1170,11 +1556,11 @@
       <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1286,11 +1672,11 @@
     </row>
     <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="67"/>
     </row>
     <row r="16" spans="2:7" s="36" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="29"/>
@@ -1340,11 +1726,11 @@
   <sheetData>
     <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="F2" s="37" t="s">
         <v>24</v>
       </c>
@@ -1458,11 +1844,11 @@
     </row>
     <row r="14" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="54"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="67"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B16" s="29"/>
@@ -1497,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE59413-D9F3-44A1-88DC-A59245E9D9B8}">
   <dimension ref="B1:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1510,11 +1896,11 @@
   <sheetData>
     <row r="1" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="67"/>
       <c r="F2" s="50" t="s">
         <v>24</v>
       </c>
@@ -1696,11 +2082,11 @@
     </row>
     <row r="22" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="53"/>
-      <c r="D23" s="54"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="67"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="29"/>
@@ -1754,6 +2140,648 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D03A187-FF98-4B1B-892D-A571F19F5DA5}">
+  <dimension ref="A1:E44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="69"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="69"/>
+      <c r="B4" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="69"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="69"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="69"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="69"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="69"/>
+      <c r="B10" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="69"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="69"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="69"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="69"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="69"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="69"/>
+      <c r="B16" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="69"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="69"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="69"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="69"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="70"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="69"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="69"/>
+      <c r="B24" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="69"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="69"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="69"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="69"/>
+      <c r="B28" s="75"/>
+      <c r="C28" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="69"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="69"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="69"/>
+      <c r="B31" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="69"/>
+      <c r="B32" s="75"/>
+      <c r="C32" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="69"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="69"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="69"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="69"/>
+      <c r="B36" s="75"/>
+      <c r="C36" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="69"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="69"/>
+      <c r="B38" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="69"/>
+      <c r="B39" s="75"/>
+      <c r="C39" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="69"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="69"/>
+      <c r="B41" s="75"/>
+      <c r="C41" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="69"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="69"/>
+      <c r="B43" s="75"/>
+      <c r="C43" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="28">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="69"/>
+      <c r="B44" s="75"/>
+      <c r="C44" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="A22:A44"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B16:B21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09720AAE-8591-438C-A715-1527441BF57F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE247F88-6DDE-433E-81AC-06E8044E24FC}">
   <dimension ref="B1:G11"/>
   <sheetViews>
@@ -1774,11 +2802,11 @@
       <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="57"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="79"/>
       <c r="F2" s="7" t="s">
         <v>24</v>
       </c>
@@ -1834,12 +2862,12 @@
     </row>
     <row r="8" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="79"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="29"/>
@@ -1877,7 +2905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53111C9A-58C1-40C7-9383-CFE5F1F570E0}">
   <dimension ref="B1:F38"/>
   <sheetViews>
@@ -1895,14 +2923,14 @@
   <sheetData>
     <row r="1" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="E2" s="58" t="s">
+      <c r="C2" s="81"/>
+      <c r="E2" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="59"/>
+      <c r="F2" s="81"/>
     </row>
     <row r="3" spans="2:6" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="18" t="s">
@@ -2329,11 +3357,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BF41A8-026E-451A-9D63-213454538E4C}">
   <dimension ref="B1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -2341,10 +3369,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="59"/>
+      <c r="C2" s="81"/>
     </row>
     <row r="3" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="18" t="s">
@@ -2550,7 +3578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EED9BCF-AC84-402D-B7FA-16D351A40D85}">
   <dimension ref="B1:C7"/>
   <sheetViews>
@@ -2565,10 +3593,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="59"/>
+      <c r="C2" s="81"/>
     </row>
     <row r="3" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="5" t="s">

</xml_diff>

<commit_message>
Fix Bernard missing water level
</commit_message>
<xml_diff>
--- a/Resources/Metadata.xlsx
+++ b/Resources/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulavaldti-my.sharepoint.com/personal/anthi182_ulaval_ca/Documents/Documents/GitHub/Ro2_data_worflow/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6983D7D3-A322-4149-A22B-9F8F3383839B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EFE9012-1AD4-4EC7-BD00-EB4AB18C122F}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{6983D7D3-A322-4149-A22B-9F8F3383839B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37BD5D76-8893-4946-A75A-CCD4E1D96557}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="5" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="5" xr2:uid="{70FED0F5-DA18-6E4C-8F4F-A74F12345264}"/>
   </bookViews>
   <sheets>
     <sheet name="Berge" sheetId="3" r:id="rId1"/>
@@ -1925,8 +1925,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3390240" y="5008252"/>
-          <a:ext cx="893124" cy="4898572"/>
+          <a:off x="3396136" y="4894860"/>
+          <a:ext cx="899474" cy="4776107"/>
           <a:chOff x="3065318" y="5264727"/>
           <a:chExt cx="1004455" cy="5143500"/>
         </a:xfrm>
@@ -2079,8 +2079,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3081811" y="6459682"/>
-          <a:ext cx="893124" cy="6168570"/>
+          <a:off x="3096779" y="6310003"/>
+          <a:ext cx="899474" cy="6014357"/>
           <a:chOff x="3065318" y="5264727"/>
           <a:chExt cx="1004455" cy="5143500"/>
         </a:xfrm>
@@ -2233,8 +2233,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1766454" y="3410856"/>
-          <a:ext cx="893124" cy="2867395"/>
+          <a:off x="1776886" y="3336924"/>
+          <a:ext cx="899474" cy="2796185"/>
           <a:chOff x="3065318" y="5264727"/>
           <a:chExt cx="1004455" cy="5143500"/>
         </a:xfrm>
@@ -2448,8 +2448,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1766454" y="6549572"/>
-          <a:ext cx="893124" cy="3720109"/>
+          <a:off x="1776886" y="6398532"/>
+          <a:ext cx="899474" cy="3626220"/>
           <a:chOff x="3065318" y="5264727"/>
           <a:chExt cx="1004455" cy="5143500"/>
         </a:xfrm>
@@ -2602,8 +2602,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2133846" y="5837464"/>
-          <a:ext cx="288225" cy="440787"/>
+          <a:off x="2144278" y="5701393"/>
+          <a:ext cx="288225" cy="431716"/>
           <a:chOff x="3065318" y="5264727"/>
           <a:chExt cx="1004455" cy="5143500"/>
         </a:xfrm>
@@ -9413,8 +9413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE59413-D9F3-44A1-88DC-A59245E9D9B8}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>